<commit_message>
Finished linear actuator assembly
</commit_message>
<xml_diff>
--- a/Lab 3/Linear Actuator Tables.xlsx
+++ b/Lab 3/Linear Actuator Tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -112,13 +112,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -213,6 +213,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -248,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,7 +437,7 @@
   <dimension ref="E4:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,43 +451,43 @@
   </cols>
   <sheetData>
     <row r="4" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="1">
@@ -473,7 +507,7 @@
       </c>
     </row>
     <row r="8" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1">
@@ -487,6 +521,9 @@
       </c>
       <c r="I8" s="1">
         <v>511</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to New version of Actuator attachments
</commit_message>
<xml_diff>
--- a/Lab 3/Linear Actuator Tables.xlsx
+++ b/Lab 3/Linear Actuator Tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -112,13 +112,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -213,6 +213,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -248,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,7 +437,7 @@
   <dimension ref="E4:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,43 +451,43 @@
   </cols>
   <sheetData>
     <row r="4" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="1">
@@ -473,7 +507,7 @@
       </c>
     </row>
     <row r="8" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1">
@@ -487,6 +521,9 @@
       </c>
       <c r="I8" s="1">
         <v>511</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created actuator panel mount drawing
</commit_message>
<xml_diff>
--- a/Lab 3/Linear Actuator Tables.xlsx
+++ b/Lab 3/Linear Actuator Tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Max Allowable</t>
   </si>
@@ -43,6 +43,36 @@
   </si>
   <si>
     <t>Rated RPM</t>
+  </si>
+  <si>
+    <t>Bolting Provisions for Motion Assembly</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Specifications</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Hex Bolt</t>
+  </si>
+  <si>
+    <t>Hex Nut</t>
+  </si>
+  <si>
+    <t>5/8"-11x2.5"</t>
+  </si>
+  <si>
+    <t>5/8"-11</t>
+  </si>
+  <si>
+    <t>1 1/4"-12x2.5"</t>
+  </si>
+  <si>
+    <t>1 1/4"-12</t>
   </si>
 </sst>
 </file>
@@ -107,7 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -117,6 +147,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -434,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:J8"/>
+  <dimension ref="E4:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,9 +481,11 @@
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
@@ -460,7 +495,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -468,7 +503,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="2" t="s">
         <v>2</v>
@@ -486,7 +521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +541,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
@@ -526,9 +561,78 @@
         <v>1450</v>
       </c>
     </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" s="1">
+        <f>12*3</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="1">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E4:J4"/>
+    <mergeCell ref="M12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>